<commit_message>
Update Excel file from PR #32
</commit_message>
<xml_diff>
--- a/.github/excel/data.xlsx
+++ b/.github/excel/data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -417,10 +417,17 @@
         <v>作業</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>#18</v>
+      </c>
+      <c r="B2" t="str">
+        <v>テスト</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Excel file from PR #33
</commit_message>
<xml_diff>
--- a/.github/excel/data.xlsx
+++ b/.github/excel/data.xlsx
@@ -1,151 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C764111-4B4C-4C29-B87C-C8DB34DFD761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="issue一覧" sheetId="1" r:id="rId1"/>
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
-  <si>
-    <t>issue番号</t>
-  </si>
-  <si>
-    <t>issueタイトル</t>
-  </si>
-  <si>
-    <t>実装時間</t>
-  </si>
-  <si>
-    <t>実装済み</t>
-  </si>
-  <si>
-    <t>レビュー時間</t>
-  </si>
-  <si>
-    <t>レビュー済み</t>
-  </si>
-  <si>
-    <t>テスト</t>
-  </si>
-  <si>
-    <t>テスト2</t>
-  </si>
-  <si>
-    <t>テスト3</t>
-  </si>
-  <si>
-    <t>テスト4</t>
-  </si>
-  <si>
-    <t>テスト5</t>
-  </si>
-  <si>
-    <t>テスト6</t>
-  </si>
-  <si>
-    <t>テスト7</t>
-  </si>
-  <si>
-    <t>テスト8</t>
-  </si>
-  <si>
-    <t>テスト9</t>
-  </si>
-  <si>
-    <t>テスト10</t>
-  </si>
-  <si>
-    <t>テスト11</t>
-  </si>
-  <si>
-    <t>テスト12</t>
-  </si>
-  <si>
-    <t>テスト13</t>
-  </si>
-  <si>
-    <t>テスト14</t>
-  </si>
-  <si>
-    <t>テスト15</t>
-  </si>
-  <si>
-    <t>テスト16</t>
-  </si>
-  <si>
-    <t>テスト17</t>
-  </si>
-  <si>
-    <t>テスト18</t>
-  </si>
-  <si>
-    <t>テスト19</t>
-  </si>
-  <si>
-    <t>テスト20</t>
-  </si>
-  <si>
-    <t>テスト21</t>
-  </si>
-  <si>
-    <t>テスト22</t>
-  </si>
-  <si>
-    <t>テスト23</t>
-  </si>
-  <si>
-    <t>テスト24</t>
-  </si>
-  <si>
-    <t>テスト25</t>
-  </si>
-  <si>
-    <t>テスト26</t>
-  </si>
-  <si>
-    <t>テスト27</t>
-  </si>
-  <si>
-    <t>Issue Number</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -179,18 +69,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -515,62 +397,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F28"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
-    <col min="2" max="2" width="26.25" customWidth="1"/>
-    <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>issue番号</v>
+      </c>
+      <c r="B1" t="str">
+        <v>issueタイトル</v>
+      </c>
+      <c r="C1" t="str">
+        <v>実装時間</v>
+      </c>
+      <c r="D1" t="str">
+        <v>実装済み</v>
+      </c>
+      <c r="E1" t="str">
+        <v>レビュー時間</v>
+      </c>
+      <c r="F1" t="str">
+        <v>レビュー済み</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" t="str">
+        <v>テスト</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
+      <c r="D2" t="str">
+        <v>済</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" t="str">
+        <v>テスト2</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -579,12 +454,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4" t="str">
+        <v>テスト3</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -593,12 +468,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5" t="str">
+        <v>テスト4</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -607,12 +482,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="B6" t="str">
+        <v>テスト5</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -621,12 +496,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7" t="str">
+        <v>テスト6</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -635,12 +510,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
+      <c r="B8" t="str">
+        <v>テスト7</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -649,12 +524,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
+      <c r="B9" t="str">
+        <v>テスト8</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -663,12 +538,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
+      <c r="B10" t="str">
+        <v>テスト9</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -677,12 +552,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
+      <c r="B11" t="str">
+        <v>テスト10</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -691,12 +566,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
+      <c r="B12" t="str">
+        <v>テスト11</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -705,12 +580,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
+      <c r="B13" t="str">
+        <v>テスト12</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -719,12 +594,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>18</v>
+      <c r="B14" t="str">
+        <v>テスト13</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -733,12 +608,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
+      <c r="B15" t="str">
+        <v>テスト14</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -747,12 +622,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
+      <c r="B16" t="str">
+        <v>テスト15</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -761,12 +636,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="A17">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
+      <c r="B17" t="str">
+        <v>テスト16</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -775,12 +650,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
-        <v>22</v>
+      <c r="B18" t="str">
+        <v>テスト17</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -789,12 +664,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="A19">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
-        <v>23</v>
+      <c r="B19" t="str">
+        <v>テスト18</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -803,12 +678,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
-        <v>24</v>
+      <c r="B20" t="str">
+        <v>テスト19</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -817,12 +692,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="A21">
         <v>37</v>
       </c>
-      <c r="B21" t="s">
-        <v>25</v>
+      <c r="B21" t="str">
+        <v>テスト20</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -831,12 +706,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
-        <v>26</v>
+      <c r="B22" t="str">
+        <v>テスト21</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -845,12 +720,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="A23">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
-        <v>27</v>
+      <c r="B23" t="str">
+        <v>テスト22</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -859,12 +734,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24">
         <v>40</v>
       </c>
-      <c r="B24" t="s">
-        <v>28</v>
+      <c r="B24" t="str">
+        <v>テスト23</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -873,12 +748,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="A25">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
+      <c r="B25" t="str">
+        <v>テスト24</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -887,12 +762,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26">
       <c r="A26">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
-        <v>30</v>
+      <c r="B26" t="str">
+        <v>テスト25</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -901,12 +776,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27">
       <c r="A27">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
-        <v>31</v>
+      <c r="B27" t="str">
+        <v>テスト26</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -915,12 +790,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28">
       <c r="A28">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
-        <v>32</v>
+      <c r="B28" t="str">
+        <v>テスト27</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -932,47 +807,46 @@
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A1" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F28"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Issue Number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Title</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B3" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>